<commit_message>
syst_c -> syst_u for E772
</commit_message>
<xml_diff>
--- a/proton_qT/expdata/10772.xlsx
+++ b/proton_qT/expdata/10772.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/proton_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2503608D-C489-2048-A857-C1EA8DADDADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8158D13-61BE-644E-A682-E94234C0E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="3700" windowWidth="28040" windowHeight="17440" xr2:uid="{E748A6B3-C705-8646-AAB9-41680F0509DB}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>H2</t>
   </si>
   <si>
-    <t>syst_c</t>
-  </si>
-  <si>
     <t>Qmin</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>pD</t>
+  </si>
+  <si>
+    <t>syst_u</t>
   </si>
 </sst>
 </file>
@@ -470,22 +470,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
@@ -570,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -625,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="Q3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="Q4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="Q5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -790,7 +790,7 @@
         <v>10</v>
       </c>
       <c r="Q6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -845,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="Q7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -900,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="Q8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -955,7 +955,7 @@
         <v>10</v>
       </c>
       <c r="Q9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1010,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="Q10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1065,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="Q11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
         <v>10</v>
       </c>
       <c r="Q12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -1175,7 +1175,7 @@
         <v>10</v>
       </c>
       <c r="Q13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1230,7 +1230,7 @@
         <v>10</v>
       </c>
       <c r="Q14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>10</v>
       </c>
       <c r="Q15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1340,7 +1340,7 @@
         <v>10</v>
       </c>
       <c r="Q16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1395,7 +1395,7 @@
         <v>10</v>
       </c>
       <c r="Q17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -1450,7 +1450,7 @@
         <v>10</v>
       </c>
       <c r="Q18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -1505,7 +1505,7 @@
         <v>10</v>
       </c>
       <c r="Q19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -1560,7 +1560,7 @@
         <v>10</v>
       </c>
       <c r="Q20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -1615,7 +1615,7 @@
         <v>10</v>
       </c>
       <c r="Q21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -1670,7 +1670,7 @@
         <v>10</v>
       </c>
       <c r="Q22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -1725,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="Q23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -1780,7 +1780,7 @@
         <v>10</v>
       </c>
       <c r="Q24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -1835,7 +1835,7 @@
         <v>10</v>
       </c>
       <c r="Q25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -1890,7 +1890,7 @@
         <v>10</v>
       </c>
       <c r="Q26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -1945,7 +1945,7 @@
         <v>10</v>
       </c>
       <c r="Q27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -2000,7 +2000,7 @@
         <v>10</v>
       </c>
       <c r="Q28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -2055,7 +2055,7 @@
         <v>10</v>
       </c>
       <c r="Q29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -2110,7 +2110,7 @@
         <v>10</v>
       </c>
       <c r="Q30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -2165,7 +2165,7 @@
         <v>10</v>
       </c>
       <c r="Q31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -2220,7 +2220,7 @@
         <v>10</v>
       </c>
       <c r="Q32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -2275,7 +2275,7 @@
         <v>10</v>
       </c>
       <c r="Q33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -2330,7 +2330,7 @@
         <v>10</v>
       </c>
       <c r="Q34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -2385,7 +2385,7 @@
         <v>10</v>
       </c>
       <c r="Q35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -2440,7 +2440,7 @@
         <v>10</v>
       </c>
       <c r="Q36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="Q37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -2550,7 +2550,7 @@
         <v>10</v>
       </c>
       <c r="Q38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -2605,7 +2605,7 @@
         <v>10</v>
       </c>
       <c r="Q39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
@@ -2660,7 +2660,7 @@
         <v>10</v>
       </c>
       <c r="Q40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -2715,7 +2715,7 @@
         <v>10</v>
       </c>
       <c r="Q41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -2770,7 +2770,7 @@
         <v>10</v>
       </c>
       <c r="Q42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -2825,7 +2825,7 @@
         <v>10</v>
       </c>
       <c r="Q43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -2880,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="Q44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
@@ -2935,7 +2935,7 @@
         <v>10</v>
       </c>
       <c r="Q45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -2990,7 +2990,7 @@
         <v>10</v>
       </c>
       <c r="Q46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -3045,7 +3045,7 @@
         <v>10</v>
       </c>
       <c r="Q47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -3100,7 +3100,7 @@
         <v>10</v>
       </c>
       <c r="Q48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -3155,7 +3155,7 @@
         <v>10</v>
       </c>
       <c r="Q49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
@@ -3210,7 +3210,7 @@
         <v>10</v>
       </c>
       <c r="Q50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -3265,7 +3265,7 @@
         <v>10</v>
       </c>
       <c r="Q51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
@@ -3320,7 +3320,7 @@
         <v>10</v>
       </c>
       <c r="Q52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -3375,7 +3375,7 @@
         <v>10</v>
       </c>
       <c r="Q53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
@@ -3430,7 +3430,7 @@
         <v>10</v>
       </c>
       <c r="Q54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
@@ -3485,7 +3485,7 @@
         <v>10</v>
       </c>
       <c r="Q55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -3540,7 +3540,7 @@
         <v>10</v>
       </c>
       <c r="Q56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -3595,7 +3595,7 @@
         <v>10</v>
       </c>
       <c r="Q57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -3650,7 +3650,7 @@
         <v>10</v>
       </c>
       <c r="Q58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
@@ -3705,7 +3705,7 @@
         <v>10</v>
       </c>
       <c r="Q59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -3760,7 +3760,7 @@
         <v>10</v>
       </c>
       <c r="Q60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -3815,7 +3815,7 @@
         <v>10</v>
       </c>
       <c r="Q61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
@@ -3870,7 +3870,7 @@
         <v>10</v>
       </c>
       <c r="Q62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -3925,7 +3925,7 @@
         <v>10</v>
       </c>
       <c r="Q63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
@@ -3980,7 +3980,7 @@
         <v>10</v>
       </c>
       <c r="Q64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -4035,7 +4035,7 @@
         <v>10</v>
       </c>
       <c r="Q65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
@@ -4090,7 +4090,7 @@
         <v>10</v>
       </c>
       <c r="Q66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
@@ -4145,7 +4145,7 @@
         <v>10</v>
       </c>
       <c r="Q67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -4200,7 +4200,7 @@
         <v>10</v>
       </c>
       <c r="Q68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -4255,7 +4255,7 @@
         <v>10</v>
       </c>
       <c r="Q69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
@@ -4310,7 +4310,7 @@
         <v>10</v>
       </c>
       <c r="Q70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -4365,7 +4365,7 @@
         <v>10</v>
       </c>
       <c r="Q71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -4420,7 +4420,7 @@
         <v>10</v>
       </c>
       <c r="Q72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
@@ -4475,7 +4475,7 @@
         <v>10</v>
       </c>
       <c r="Q73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
@@ -4530,7 +4530,7 @@
         <v>10</v>
       </c>
       <c r="Q74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -4585,7 +4585,7 @@
         <v>10</v>
       </c>
       <c r="Q75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
@@ -4640,7 +4640,7 @@
         <v>10</v>
       </c>
       <c r="Q76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
@@ -4695,7 +4695,7 @@
         <v>10</v>
       </c>
       <c r="Q77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -4750,7 +4750,7 @@
         <v>10</v>
       </c>
       <c r="Q78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
@@ -4805,7 +4805,7 @@
         <v>10</v>
       </c>
       <c r="Q79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
@@ -4860,7 +4860,7 @@
         <v>10</v>
       </c>
       <c r="Q80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -4915,7 +4915,7 @@
         <v>10</v>
       </c>
       <c r="Q81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
@@ -4970,7 +4970,7 @@
         <v>10</v>
       </c>
       <c r="Q82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
@@ -5025,7 +5025,7 @@
         <v>10</v>
       </c>
       <c r="Q83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
@@ -5080,7 +5080,7 @@
         <v>10</v>
       </c>
       <c r="Q84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
@@ -5135,7 +5135,7 @@
         <v>10</v>
       </c>
       <c r="Q85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
@@ -5190,7 +5190,7 @@
         <v>10</v>
       </c>
       <c r="Q86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
@@ -5245,7 +5245,7 @@
         <v>10</v>
       </c>
       <c r="Q87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -5300,7 +5300,7 @@
         <v>10</v>
       </c>
       <c r="Q88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -5355,7 +5355,7 @@
         <v>10</v>
       </c>
       <c r="Q89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -5410,7 +5410,7 @@
         <v>10</v>
       </c>
       <c r="Q90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -5465,7 +5465,7 @@
         <v>10</v>
       </c>
       <c r="Q91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -5520,7 +5520,7 @@
         <v>10</v>
       </c>
       <c r="Q92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Q ranges in E772 correctly
</commit_message>
<xml_diff>
--- a/proton_qT/expdata/10772.xlsx
+++ b/proton_qT/expdata/10772.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/proton_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8158D13-61BE-644E-A682-E94234C0E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA541DE2-9523-C54E-BED9-D22438444E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="3700" windowWidth="28040" windowHeight="17440" xr2:uid="{E748A6B3-C705-8646-AAB9-41680F0509DB}"/>
   </bookViews>
@@ -3603,10 +3603,10 @@
         <v>800</v>
       </c>
       <c r="B58">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C58">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>0.1</v>
@@ -3658,10 +3658,10 @@
         <v>800</v>
       </c>
       <c r="B59">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D59">
         <v>0.1</v>
@@ -3713,10 +3713,10 @@
         <v>800</v>
       </c>
       <c r="B60">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D60">
         <v>0.1</v>
@@ -3768,10 +3768,10 @@
         <v>800</v>
       </c>
       <c r="B61">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C61">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D61">
         <v>0.1</v>
@@ -3823,10 +3823,10 @@
         <v>800</v>
       </c>
       <c r="B62">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C62">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D62">
         <v>0.1</v>
@@ -3878,10 +3878,10 @@
         <v>800</v>
       </c>
       <c r="B63">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C63">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D63">
         <v>0.1</v>
@@ -3933,10 +3933,10 @@
         <v>800</v>
       </c>
       <c r="B64">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D64">
         <v>0.1</v>
@@ -3988,10 +3988,10 @@
         <v>800</v>
       </c>
       <c r="B65">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C65">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>0.1</v>
@@ -4043,10 +4043,10 @@
         <v>800</v>
       </c>
       <c r="B66">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C66">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D66">
         <v>0.1</v>
@@ -4098,10 +4098,10 @@
         <v>800</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C67">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D67">
         <v>0.1</v>
@@ -4153,10 +4153,10 @@
         <v>800</v>
       </c>
       <c r="B68">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D68">
         <v>0.1</v>

</xml_diff>